<commit_message>
Work done on results and conclusions section. Added some new graphs. Made some great points etc. Just panic commited because my battery got low.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="43">
   <si>
     <t>Image Dimensions</t>
   </si>
@@ -162,6 +162,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,7 +798,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -846,18 +849,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -912,6 +903,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2691,7 +2703,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2704,14 +2716,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Parallel</a:t>
+              <a:rPr lang="en-GB" sz="2400" baseline="0"/>
+              <a:t>Parallel Algorithm Performance: 4 vs 8 Threads</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Algorithm Performance: 4 vs 8 Threads</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2728,7 +2735,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2746,7 +2753,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.229502265307063E-2"/>
+          <c:y val="0.10235678130891536"/>
+          <c:w val="0.90770497734692934"/>
+          <c:h val="0.77499149381910726"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2768,6 +2785,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2782,7 +2800,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2883,6 +2901,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2897,7 +2916,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3024,7 +3043,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3074,7 +3093,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3087,7 +3106,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0"/>
                   <a:t>Average Time / ms</a:t>
                 </a:r>
               </a:p>
@@ -3106,7 +3125,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3138,7 +3157,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3167,6 +3186,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33888487833191727"/>
+          <c:y val="0.94387735687285867"/>
+          <c:w val="0.32223012785060234"/>
+          <c:h val="5.6122643127141172E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3180,7 +3209,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3205,12 +3234,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -5464,7 +5488,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="97" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5475,7 +5499,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662276" cy="6279931"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5508,7 +5532,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662276" cy="6279931"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5541,7 +5565,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662276" cy="6279931"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5868,8 +5892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5885,27 +5909,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="R1" s="43" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="R1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="W1" s="22" t="s">
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="W1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5986,25 +6010,25 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
       <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
       <c r="V3" s="11"/>
       <c r="W3" s="7">
         <v>1</v>
@@ -6238,7 +6262,7 @@
       <c r="U7" s="1">
         <v>48115</v>
       </c>
-      <c r="W7" s="31">
+      <c r="W7" s="27">
         <v>1</v>
       </c>
       <c r="X7" s="1">
@@ -6302,7 +6326,7 @@
       <c r="U8" s="1">
         <v>48483</v>
       </c>
-      <c r="W8" s="31">
+      <c r="W8" s="27">
         <v>2</v>
       </c>
       <c r="X8" s="1">
@@ -6366,7 +6390,7 @@
       <c r="U9" s="1">
         <v>47987</v>
       </c>
-      <c r="W9" s="31">
+      <c r="W9" s="27">
         <v>3</v>
       </c>
       <c r="X9" s="1">
@@ -6430,10 +6454,10 @@
       <c r="U10" s="1">
         <v>48089</v>
       </c>
-      <c r="W10" s="24"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -6480,7 +6504,7 @@
       <c r="U11" s="1">
         <v>48173</v>
       </c>
-      <c r="W11" s="24"/>
+      <c r="W11" s="20"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
@@ -6529,16 +6553,16 @@
       <c r="U12" s="1">
         <v>47788</v>
       </c>
-      <c r="W12" s="26"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="39"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7">
         <v>10</v>
@@ -6582,10 +6606,10 @@
       <c r="U13" s="1">
         <v>47748</v>
       </c>
-      <c r="W13" s="26"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -10712,8 +10736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10729,27 +10753,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="R1" s="43" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="R1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="W1" s="22" t="s">
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="W1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -10805,7 +10829,7 @@
       <c r="U2" s="12">
         <v>1024</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="W2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="X2" s="15" t="s">
@@ -10830,25 +10854,25 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
       <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
       <c r="W3" s="7">
         <v>1</v>
       </c>
@@ -11330,10 +11354,10 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="39"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7">
         <v>10</v>
@@ -11779,11 +11803,11 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="E22" s="1"/>
       <c r="F22" s="7">
         <v>19</v>
@@ -11886,11 +11910,11 @@
       <c r="A24" s="7">
         <v>4</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="41">
         <f>'Seq. Results'!B3/'OpenMP Static'!B3</f>
         <v>4.0750814941484537</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="42">
         <f>B24/B20</f>
         <v>1.0187703735371134</v>
       </c>
@@ -11942,11 +11966,11 @@
       <c r="A25" s="7">
         <v>8</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="41">
         <f>'Seq. Results'!B4/'OpenMP Static'!B4</f>
         <v>4.1191280566280568</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="43">
         <f>B25/B20</f>
         <v>1.0297820141570142</v>
       </c>
@@ -11998,11 +12022,11 @@
       <c r="A26" s="7">
         <v>16</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="41">
         <f>'Seq. Results'!B5/'OpenMP Static'!B5</f>
         <v>4.2025957972805932</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="43">
         <f>B26/B20</f>
         <v>1.0506489493201483</v>
       </c>
@@ -12054,11 +12078,11 @@
       <c r="A27" s="7">
         <v>32</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="41">
         <f>'Seq. Results'!B6/'OpenMP Static'!B6</f>
         <v>4.3582268286704711</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="43">
         <f>B27/B20</f>
         <v>1.0895567071676178</v>
       </c>
@@ -12110,11 +12134,11 @@
       <c r="A28" s="7">
         <v>64</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="41">
         <f>'Seq. Results'!B7/'OpenMP Static'!B7</f>
         <v>4.4610101802492474</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="43">
         <f>B28/B20</f>
         <v>1.1152525450623119</v>
       </c>
@@ -12166,11 +12190,11 @@
       <c r="A29" s="7">
         <v>128</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="41">
         <f>'Seq. Results'!B8/'OpenMP Static'!B8</f>
         <v>4.3909204262680435</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="43">
         <f>B29/B20</f>
         <v>1.0977301065670109</v>
       </c>
@@ -12222,11 +12246,11 @@
       <c r="A30" s="7">
         <v>256</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="41">
         <f>'Seq. Results'!B9/'OpenMP Static'!B9</f>
         <v>4.3285418654617702</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="43">
         <f>B30/B20</f>
         <v>1.0821354663654426</v>
       </c>
@@ -12278,11 +12302,11 @@
       <c r="A31" s="7">
         <v>512</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="41">
         <f>'Seq. Results'!B10/'OpenMP Static'!B10</f>
         <v>4.302667827213436</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="43">
         <f>B31/B20</f>
         <v>1.075666956803359</v>
       </c>
@@ -12376,11 +12400,11 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="E33" s="1"/>
       <c r="F33" s="7">
         <v>30</v>
@@ -12483,11 +12507,11 @@
       <c r="A35" s="7">
         <v>128</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="45">
         <f>'Seq. Results'!B15/'OpenMP Static'!B15</f>
         <v>3.9862201570261182</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="41">
         <f>B35/B20</f>
         <v>0.99655503925652955</v>
       </c>
@@ -12539,11 +12563,11 @@
       <c r="A36" s="7">
         <v>256</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="46">
         <f>'Seq. Results'!B16/'OpenMP Static'!B16</f>
         <v>4.1328000658580759</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="41">
         <f>B36/B20</f>
         <v>1.033200016464519</v>
       </c>
@@ -12595,11 +12619,11 @@
       <c r="A37" s="7">
         <v>512</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B37" s="46">
         <f>'Seq. Results'!B17/'OpenMP Static'!B17</f>
         <v>4.2167345721951701</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="41">
         <f>B37/B20</f>
         <v>1.0541836430487925</v>
       </c>
@@ -12651,11 +12675,11 @@
       <c r="A38" s="7">
         <v>1024</v>
       </c>
-      <c r="B38" s="21">
+      <c r="B38" s="46">
         <f>'Seq. Results'!B18/'OpenMP Static'!B18</f>
         <v>4.3117982336797374</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="41">
         <f>B38/B20</f>
         <v>1.0779495584199343</v>
       </c>
@@ -15649,7 +15673,7 @@
   <dimension ref="A1:Z103"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15665,35 +15689,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="R1" s="43" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="R1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="W1" s="22" t="s">
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="W1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -15741,16 +15765,16 @@
       <c r="U2" s="12">
         <v>1024</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="W2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="X2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="29" t="s">
+      <c r="Y2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="Z2" s="29" t="s">
+      <c r="Z2" s="25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15766,25 +15790,25 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
       <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
       <c r="W3" s="7">
         <v>1</v>
       </c>
@@ -16266,10 +16290,10 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="39"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7">
         <v>10</v>
@@ -16318,7 +16342,7 @@
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="1"/>
@@ -16715,11 +16739,11 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="E22" s="1"/>
       <c r="F22" s="7">
         <v>19</v>
@@ -16765,7 +16789,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -16822,11 +16846,11 @@
       <c r="A24" s="7">
         <v>4</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="41">
         <f>'Seq. Results'!B3/'OpenMP Dynamic'!B3</f>
         <v>4.6503841931942924</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="42">
         <f>B24/B20</f>
         <v>1.1625960482985731</v>
       </c>
@@ -16878,11 +16902,11 @@
       <c r="A25" s="7">
         <v>8</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="41">
         <f>'Seq. Results'!B4/'OpenMP Dynamic'!B4</f>
         <v>4.6732067895601386</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="43">
         <f>B25/B20</f>
         <v>1.1683016973900346</v>
       </c>
@@ -16934,11 +16958,11 @@
       <c r="A26" s="7">
         <v>16</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="41">
         <f>'Seq. Results'!B5/'OpenMP Dynamic'!B5</f>
         <v>4.6688384015624287</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="43">
         <f>B26/B20</f>
         <v>1.1672096003906072</v>
       </c>
@@ -16990,11 +17014,11 @@
       <c r="A27" s="7">
         <v>32</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="41">
         <f>'Seq. Results'!B6/'OpenMP Dynamic'!B6</f>
         <v>4.7553889767630224</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="43">
         <f>B27/B20</f>
         <v>1.1888472441907556</v>
       </c>
@@ -17046,11 +17070,11 @@
       <c r="A28" s="7">
         <v>64</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="41">
         <f>'Seq. Results'!B7/'OpenMP Dynamic'!B7</f>
         <v>4.7642672719102492</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="43">
         <f>B28/B20</f>
         <v>1.1910668179775623</v>
       </c>
@@ -17102,11 +17126,11 @@
       <c r="A29" s="7">
         <v>128</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="41">
         <f>'Seq. Results'!B8/'OpenMP Dynamic'!B8</f>
         <v>4.7145422765164611</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="43">
         <f>B29/B20</f>
         <v>1.1786355691291153</v>
       </c>
@@ -17152,11 +17176,11 @@
       <c r="A30" s="7">
         <v>256</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="41">
         <f>'Seq. Results'!B9/'OpenMP Dynamic'!B9</f>
         <v>4.6483652757764116</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="43">
         <f>B30/B20</f>
         <v>1.1620913189441029</v>
       </c>
@@ -17202,11 +17226,11 @@
       <c r="A31" s="7">
         <v>512</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="41">
         <f>'Seq. Results'!B10/'OpenMP Dynamic'!B10</f>
         <v>4.6163320849519645</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="43">
         <f>B31/B20</f>
         <v>1.1540830212379911</v>
       </c>
@@ -17288,11 +17312,11 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="E33" s="1"/>
       <c r="F33" s="7">
         <v>30</v>
@@ -17383,11 +17407,11 @@
       <c r="A35" s="7">
         <v>128</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="45">
         <f>'Seq. Results'!B15/'OpenMP Dynamic'!B15</f>
         <v>4.5011760448706353</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="41">
         <f>B35/B20</f>
         <v>1.1252940112176588</v>
       </c>
@@ -17433,11 +17457,11 @@
       <c r="A36" s="7">
         <v>256</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="46">
         <f>'Seq. Results'!B16/'OpenMP Dynamic'!B16</f>
         <v>4.6038332798385992</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="41">
         <f>B36/B20</f>
         <v>1.1509583199596498</v>
       </c>
@@ -17483,11 +17507,11 @@
       <c r="A37" s="7">
         <v>512</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B37" s="46">
         <f>'Seq. Results'!B17/'OpenMP Dynamic'!B17</f>
         <v>4.6000681420451901</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="41">
         <f>B37/B20</f>
         <v>1.1500170355112975</v>
       </c>
@@ -17533,11 +17557,11 @@
       <c r="A38" s="7">
         <v>1024</v>
       </c>
-      <c r="B38" s="21">
+      <c r="B38" s="46">
         <f>'Seq. Results'!B18/'OpenMP Dynamic'!B18</f>
         <v>4.6539923288779619</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="41">
         <f>B38/B20</f>
         <v>1.1634980822194905</v>
       </c>
@@ -20033,8 +20057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20050,35 +20074,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="R1" s="43" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="R1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="W1" s="22" t="s">
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="W1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -20126,16 +20150,16 @@
       <c r="U2" s="12">
         <v>1024</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="W2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="X2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="29" t="s">
+      <c r="Y2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="Z2" s="29" t="s">
+      <c r="Z2" s="25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -20151,25 +20175,25 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
       <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
       <c r="W3" s="7">
         <v>1</v>
       </c>
@@ -20651,10 +20675,10 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="39"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7">
         <v>10</v>
@@ -20703,7 +20727,7 @@
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="1"/>
@@ -21100,11 +21124,11 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="E22" s="1"/>
       <c r="F22" s="7">
         <v>19</v>
@@ -21150,7 +21174,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -21207,11 +21231,11 @@
       <c r="A24" s="7">
         <v>4</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="41">
         <f>'Seq. Results'!B3/'Manual Threading'!B3</f>
         <v>4.515722153135548</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="42">
         <f>B24/B20</f>
         <v>1.128930538283887</v>
       </c>
@@ -21263,11 +21287,11 @@
       <c r="A25" s="7">
         <v>8</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="41">
         <f>'Seq. Results'!B4/'Manual Threading'!B4</f>
         <v>4.6029182646212847</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="43">
         <f>B25/B20</f>
         <v>1.1507295661553212</v>
       </c>
@@ -21319,11 +21343,11 @@
       <c r="A26" s="7">
         <v>16</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="41">
         <f>'Seq. Results'!B5/'Manual Threading'!B5</f>
         <v>4.7106701356281846</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="43">
         <f>B26/B20</f>
         <v>1.1776675339070461</v>
       </c>
@@ -21375,11 +21399,11 @@
       <c r="A27" s="7">
         <v>32</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="41">
         <f>'Seq. Results'!B6/'Manual Threading'!B6</f>
         <v>4.8492850742198153</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="43">
         <f>B27/B20</f>
         <v>1.2123212685549538</v>
       </c>
@@ -21431,11 +21455,11 @@
       <c r="A28" s="7">
         <v>64</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="41">
         <f>'Seq. Results'!B7/'Manual Threading'!B7</f>
         <v>4.8671166527261764</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="43">
         <f>B28/B20</f>
         <v>1.2167791631815441</v>
       </c>
@@ -21487,11 +21511,11 @@
       <c r="A29" s="7">
         <v>128</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="41">
         <f>'Seq. Results'!B8/'Manual Threading'!B8</f>
         <v>4.8120552081086911</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="43">
         <f>B29/B20</f>
         <v>1.2030138020271728</v>
       </c>
@@ -21537,11 +21561,11 @@
       <c r="A30" s="7">
         <v>256</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="41">
         <f>'Seq. Results'!B9/'Manual Threading'!B9</f>
         <v>4.7611160133111214</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="43">
         <f>B30/B20</f>
         <v>1.1902790033277804</v>
       </c>
@@ -21587,11 +21611,11 @@
       <c r="A31" s="7">
         <v>512</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="41">
         <f>'Seq. Results'!B10/'Manual Threading'!B10</f>
         <v>4.6812327506899729</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="43">
         <f>B31/B20</f>
         <v>1.1703081876724932</v>
       </c>
@@ -21673,11 +21697,11 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="E33" s="1"/>
       <c r="F33" s="7">
         <v>30</v>
@@ -21720,7 +21744,7 @@
       <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="16" t="s">
@@ -21768,11 +21792,11 @@
       <c r="A35" s="6">
         <v>128</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="44">
         <f>'Seq. Results'!B15/'Manual Threading'!B15</f>
         <v>4.4314214463840402</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="42">
         <f>B35/B20</f>
         <v>1.1078553615960101</v>
       </c>
@@ -21818,11 +21842,11 @@
       <c r="A36" s="7">
         <v>256</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B36" s="44">
         <f>'Seq. Results'!B16/'Manual Threading'!B16</f>
         <v>4.6639260497956148</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="43">
         <f>B36/B20</f>
         <v>1.1659815124489037</v>
       </c>
@@ -21868,11 +21892,11 @@
       <c r="A37" s="7">
         <v>512</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B37" s="44">
         <f>'Seq. Results'!B17/'Manual Threading'!B17</f>
         <v>4.6031335234316888</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="43">
         <f>B37/B20</f>
         <v>1.1507833808579222</v>
       </c>
@@ -21918,11 +21942,11 @@
       <c r="A38" s="7">
         <v>1024</v>
       </c>
-      <c r="B38" s="26">
+      <c r="B38" s="44">
         <f>'Seq. Results'!B18/'Manual Threading'!B18</f>
         <v>4.6958971480606344</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="43">
         <f>B38/B20</f>
         <v>1.1739742870151586</v>
       </c>
@@ -24419,7 +24443,7 @@
   <dimension ref="A1:BB162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24434,19 +24458,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="31"/>
       <c r="K2" t="s">
         <v>25</v>
       </c>
@@ -24503,7 +24527,7 @@
       <c r="C3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="29"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
@@ -24527,10 +24551,10 @@
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="35">
         <f>AVERAGE('Seq. Results'!K4:K103)</f>
         <v>12510.68</v>
       </c>
@@ -24672,10 +24696,10 @@
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="35">
         <f>AVERAGE(AH5:AH54)</f>
         <v>11957.8</v>
       </c>
@@ -24797,10 +24821,10 @@
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="36">
         <f>AVERAGE(AC5:AC54)</f>
         <v>11770.06</v>
       </c>
@@ -24922,10 +24946,10 @@
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="35">
         <f>AVERAGE(X5:X54)</f>
         <v>8788.6200000000008</v>
       </c>
@@ -25047,8 +25071,8 @@
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="K8" s="1">
         <v>4</v>
       </c>
@@ -25285,12 +25309,12 @@
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="34"/>
       <c r="K10" s="1">
         <v>6</v>
       </c>
@@ -25418,7 +25442,7 @@
       <c r="D11" s="2">
         <v>8</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="31"/>
       <c r="K11" s="1">
         <v>7</v>
       </c>
@@ -25540,11 +25564,11 @@
       <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="34"/>
       <c r="K12" s="1">
         <v>8</v>
       </c>
@@ -25663,7 +25687,7 @@
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="1">
@@ -25793,7 +25817,7 @@
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="1">
@@ -25923,7 +25947,7 @@
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="1">
@@ -26169,7 +26193,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="17" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K17" s="1">
         <v>13</v>
       </c>
@@ -26287,7 +26311,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="18" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K18" s="1">
         <v>14</v>
       </c>
@@ -26405,7 +26429,10 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="19" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:54" x14ac:dyDescent="0.3">
+      <c r="B19" s="40" t="s">
+        <v>35</v>
+      </c>
       <c r="K19" s="1">
         <v>15</v>
       </c>
@@ -26523,7 +26550,10 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="20" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:54" x14ac:dyDescent="0.3">
+      <c r="B20" s="33" t="s">
+        <v>37</v>
+      </c>
       <c r="K20" s="1">
         <v>16</v>
       </c>
@@ -26641,7 +26671,10 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="21" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:54" x14ac:dyDescent="0.3">
+      <c r="B21" s="33" t="s">
+        <v>38</v>
+      </c>
       <c r="K21" s="1">
         <v>17</v>
       </c>
@@ -26759,7 +26792,10 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="22" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:54" x14ac:dyDescent="0.3">
+      <c r="B22" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="K22" s="1">
         <v>18</v>
       </c>
@@ -26877,7 +26913,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="23" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K23" s="1">
         <v>19</v>
       </c>
@@ -26995,7 +27031,7 @@
         <v>2588</v>
       </c>
     </row>
-    <row r="24" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K24" s="1">
         <v>20</v>
       </c>
@@ -27113,7 +27149,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="25" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K25" s="1">
         <v>21</v>
       </c>
@@ -27231,7 +27267,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="26" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K26" s="1">
         <v>22</v>
       </c>
@@ -27349,7 +27385,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="27" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K27" s="1">
         <v>23</v>
       </c>
@@ -27467,7 +27503,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="28" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K28" s="1">
         <v>24</v>
       </c>
@@ -27585,7 +27621,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="29" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K29" s="1">
         <v>25</v>
       </c>
@@ -27703,7 +27739,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="30" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K30" s="1">
         <v>26</v>
       </c>
@@ -27821,7 +27857,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="31" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K31" s="1">
         <v>27</v>
       </c>
@@ -27939,7 +27975,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="32" spans="11:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:54" x14ac:dyDescent="0.3">
       <c r="K32" s="1">
         <v>28</v>
       </c>

</xml_diff>